<commit_message>
CartPage method fix commit
</commit_message>
<xml_diff>
--- a/FinalProject/data/pet-store-data.xlsx
+++ b/FinalProject/data/pet-store-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="815">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -2161,6 +2161,306 @@
   </si>
   <si>
     <t>ce86da33</t>
+  </si>
+  <si>
+    <t>32bfe2b5</t>
+  </si>
+  <si>
+    <t>0f9df438</t>
+  </si>
+  <si>
+    <t>e32fcf25</t>
+  </si>
+  <si>
+    <t>6c2d7427</t>
+  </si>
+  <si>
+    <t>4cf52558</t>
+  </si>
+  <si>
+    <t>be13d929</t>
+  </si>
+  <si>
+    <t>ec0e533f</t>
+  </si>
+  <si>
+    <t>28c117fc</t>
+  </si>
+  <si>
+    <t>e82de048</t>
+  </si>
+  <si>
+    <t>7db6764a</t>
+  </si>
+  <si>
+    <t>edf1befd</t>
+  </si>
+  <si>
+    <t>fcd247ad</t>
+  </si>
+  <si>
+    <t>65272f08</t>
+  </si>
+  <si>
+    <t>675c1c38</t>
+  </si>
+  <si>
+    <t>50a62e6c</t>
+  </si>
+  <si>
+    <t>dc9def92</t>
+  </si>
+  <si>
+    <t>471b2f44</t>
+  </si>
+  <si>
+    <t>9907cbf4</t>
+  </si>
+  <si>
+    <t>86f94f53</t>
+  </si>
+  <si>
+    <t>970304e2</t>
+  </si>
+  <si>
+    <t>51083ca1</t>
+  </si>
+  <si>
+    <t>bfd9a0cf</t>
+  </si>
+  <si>
+    <t>129c041f</t>
+  </si>
+  <si>
+    <t>6fb90e11</t>
+  </si>
+  <si>
+    <t>f01bd949</t>
+  </si>
+  <si>
+    <t>8d3f1803</t>
+  </si>
+  <si>
+    <t>25efd4e6</t>
+  </si>
+  <si>
+    <t>b6e613b1</t>
+  </si>
+  <si>
+    <t>d1883a72</t>
+  </si>
+  <si>
+    <t>ec470243</t>
+  </si>
+  <si>
+    <t>b019d052</t>
+  </si>
+  <si>
+    <t>633bcd33</t>
+  </si>
+  <si>
+    <t>29d1c446</t>
+  </si>
+  <si>
+    <t>8ed77220</t>
+  </si>
+  <si>
+    <t>74daef1f</t>
+  </si>
+  <si>
+    <t>86e2deb6</t>
+  </si>
+  <si>
+    <t>9346fc19</t>
+  </si>
+  <si>
+    <t>c1fa0efd</t>
+  </si>
+  <si>
+    <t>1071ec73</t>
+  </si>
+  <si>
+    <t>32f158f8</t>
+  </si>
+  <si>
+    <t>83535eb6</t>
+  </si>
+  <si>
+    <t>ec08b2d5</t>
+  </si>
+  <si>
+    <t>38866a12</t>
+  </si>
+  <si>
+    <t>5579b304</t>
+  </si>
+  <si>
+    <t>6351a9da</t>
+  </si>
+  <si>
+    <t>a0737584</t>
+  </si>
+  <si>
+    <t>8aecef67</t>
+  </si>
+  <si>
+    <t>9ba98b4d</t>
+  </si>
+  <si>
+    <t>a9a8873e</t>
+  </si>
+  <si>
+    <t>1f9198ac</t>
+  </si>
+  <si>
+    <t>9384702a</t>
+  </si>
+  <si>
+    <t>06e70e3a</t>
+  </si>
+  <si>
+    <t>c3b16923</t>
+  </si>
+  <si>
+    <t>3cba4514</t>
+  </si>
+  <si>
+    <t>2202a7bd</t>
+  </si>
+  <si>
+    <t>c6240f5e</t>
+  </si>
+  <si>
+    <t>cd247874</t>
+  </si>
+  <si>
+    <t>165f6259</t>
+  </si>
+  <si>
+    <t>75e4d446</t>
+  </si>
+  <si>
+    <t>03bcf857</t>
+  </si>
+  <si>
+    <t>63298ed8</t>
+  </si>
+  <si>
+    <t>a1fb7d9b</t>
+  </si>
+  <si>
+    <t>5dccde57</t>
+  </si>
+  <si>
+    <t>4525f6ee</t>
+  </si>
+  <si>
+    <t>da83814f</t>
+  </si>
+  <si>
+    <t>80b4c93b</t>
+  </si>
+  <si>
+    <t>53a1f3d2</t>
+  </si>
+  <si>
+    <t>2cde6e96</t>
+  </si>
+  <si>
+    <t>cf308c06</t>
+  </si>
+  <si>
+    <t>0b54e04a</t>
+  </si>
+  <si>
+    <t>6778b084</t>
+  </si>
+  <si>
+    <t>e4abec67</t>
+  </si>
+  <si>
+    <t>c24ad56c</t>
+  </si>
+  <si>
+    <t>50ce42f7</t>
+  </si>
+  <si>
+    <t>7da8bde3</t>
+  </si>
+  <si>
+    <t>a58e73db</t>
+  </si>
+  <si>
+    <t>70430bdd</t>
+  </si>
+  <si>
+    <t>f9ea08e2</t>
+  </si>
+  <si>
+    <t>03d3834b</t>
+  </si>
+  <si>
+    <t>f7d7c5b7</t>
+  </si>
+  <si>
+    <t>62991d2e</t>
+  </si>
+  <si>
+    <t>eae72c4d</t>
+  </si>
+  <si>
+    <t>9d6ce120</t>
+  </si>
+  <si>
+    <t>534e98e4</t>
+  </si>
+  <si>
+    <t>fe5c8ae6</t>
+  </si>
+  <si>
+    <t>3f6c8015</t>
+  </si>
+  <si>
+    <t>c89879cc</t>
+  </si>
+  <si>
+    <t>91254d01</t>
+  </si>
+  <si>
+    <t>fc890919</t>
+  </si>
+  <si>
+    <t>510cb503</t>
+  </si>
+  <si>
+    <t>d98fdbf7</t>
+  </si>
+  <si>
+    <t>a3549972</t>
+  </si>
+  <si>
+    <t>0795cd3e</t>
+  </si>
+  <si>
+    <t>e8e60d2e</t>
+  </si>
+  <si>
+    <t>a26dd3b6</t>
+  </si>
+  <si>
+    <t>57b476a7</t>
+  </si>
+  <si>
+    <t>359cf14d</t>
+  </si>
+  <si>
+    <t>bf3a8843</t>
+  </si>
+  <si>
+    <t>89c2d2f6</t>
+  </si>
+  <si>
+    <t>2e492def</t>
   </si>
 </sst>
 </file>
@@ -2797,7 +3097,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1">
       <c r="A2" s="4" t="s">
-        <v>665</v>
+        <v>765</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2835,7 +3135,7 @@
     </row>
     <row r="3" spans="1:12" ht="30" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>666</v>
+        <v>766</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2873,7 +3173,7 @@
     </row>
     <row r="4" spans="1:12" ht="30" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>667</v>
+        <v>767</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2911,7 +3211,7 @@
     </row>
     <row r="5" spans="1:12" ht="30" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>668</v>
+        <v>768</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2949,7 +3249,7 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>669</v>
+        <v>769</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2987,7 +3287,7 @@
     </row>
     <row r="7" spans="1:12" ht="30" thickBot="1">
       <c r="A7" s="7" t="s">
-        <v>670</v>
+        <v>770</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -3025,7 +3325,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>671</v>
+        <v>771</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -3063,7 +3363,7 @@
     </row>
     <row r="9" spans="1:12" ht="30" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>672</v>
+        <v>772</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -3101,7 +3401,7 @@
     </row>
     <row r="10" spans="1:12" ht="30" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>673</v>
+        <v>773</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -3139,7 +3439,7 @@
     </row>
     <row r="11" spans="1:12" ht="30" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>674</v>
+        <v>774</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -3177,7 +3477,7 @@
     </row>
     <row r="12" spans="1:12" ht="30" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>675</v>
+        <v>775</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -3215,7 +3515,7 @@
     </row>
     <row r="13" spans="1:12" ht="30" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>676</v>
+        <v>776</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -3253,7 +3553,7 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>677</v>
+        <v>777</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -3291,7 +3591,7 @@
     </row>
     <row r="15" spans="1:12" ht="30" thickBot="1">
       <c r="A15" s="4" t="s">
-        <v>678</v>
+        <v>778</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -3329,7 +3629,7 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>679</v>
+        <v>779</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3367,7 +3667,7 @@
     </row>
     <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>680</v>
+        <v>780</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -3405,7 +3705,7 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>681</v>
+        <v>781</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -3443,7 +3743,7 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1">
       <c r="A19" s="7" t="s">
-        <v>682</v>
+        <v>782</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3481,7 +3781,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1">
       <c r="A20" s="4" t="s">
-        <v>683</v>
+        <v>783</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3519,7 +3819,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1">
       <c r="A21" s="4" t="s">
-        <v>684</v>
+        <v>784</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -3557,7 +3857,7 @@
     </row>
     <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>685</v>
+        <v>785</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -3595,7 +3895,7 @@
     </row>
     <row r="23" spans="1:12" ht="30" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>686</v>
+        <v>786</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3633,7 +3933,7 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>687</v>
+        <v>787</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3671,7 +3971,7 @@
     </row>
     <row r="25" spans="1:12" ht="30" thickBot="1">
       <c r="A25" s="7" t="s">
-        <v>688</v>
+        <v>788</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -3709,7 +4009,7 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1">
       <c r="A26" s="4" t="s">
-        <v>689</v>
+        <v>789</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -3747,7 +4047,7 @@
     </row>
     <row r="27" spans="1:12" ht="30" thickBot="1">
       <c r="A27" s="4" t="s">
-        <v>690</v>
+        <v>790</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3785,7 +4085,7 @@
     </row>
     <row r="28" spans="1:12" ht="30" thickBot="1">
       <c r="A28" s="7" t="s">
-        <v>691</v>
+        <v>791</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3823,7 +4123,7 @@
     </row>
     <row r="29" spans="1:12" ht="30" thickBot="1">
       <c r="A29" s="4" t="s">
-        <v>692</v>
+        <v>792</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3861,7 +4161,7 @@
     </row>
     <row r="30" spans="1:12" ht="30" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>693</v>
+        <v>793</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3899,7 +4199,7 @@
     </row>
     <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="7" t="s">
-        <v>694</v>
+        <v>794</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3937,7 +4237,7 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" thickBot="1">
       <c r="A32" s="4" t="s">
-        <v>695</v>
+        <v>795</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3975,7 +4275,7 @@
     </row>
     <row r="33" spans="1:12" ht="30" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>696</v>
+        <v>796</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -4013,7 +4313,7 @@
     </row>
     <row r="34" spans="1:12" ht="30" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>697</v>
+        <v>797</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -4051,7 +4351,7 @@
     </row>
     <row r="35" spans="1:12" ht="30" thickBot="1">
       <c r="A35" s="4" t="s">
-        <v>698</v>
+        <v>798</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -4089,7 +4389,7 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" thickBot="1">
       <c r="A36" s="4" t="s">
-        <v>699</v>
+        <v>799</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -4127,7 +4427,7 @@
     </row>
     <row r="37" spans="1:12" ht="30" thickBot="1">
       <c r="A37" s="7" t="s">
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -4165,7 +4465,7 @@
     </row>
     <row r="38" spans="1:12" ht="30" thickBot="1">
       <c r="A38" s="4" t="s">
-        <v>701</v>
+        <v>801</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -4203,7 +4503,7 @@
     </row>
     <row r="39" spans="1:12" ht="30" thickBot="1">
       <c r="A39" s="4" t="s">
-        <v>702</v>
+        <v>802</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -4241,7 +4541,7 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" thickBot="1">
       <c r="A40" s="7" t="s">
-        <v>703</v>
+        <v>803</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -4279,7 +4579,7 @@
     </row>
     <row r="41" spans="1:12" ht="30" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>704</v>
+        <v>804</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -4317,7 +4617,7 @@
     </row>
     <row r="42" spans="1:12" ht="30" thickBot="1">
       <c r="A42" s="4" t="s">
-        <v>705</v>
+        <v>805</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -4355,7 +4655,7 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1">
       <c r="A43" s="7" t="s">
-        <v>706</v>
+        <v>806</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -4393,7 +4693,7 @@
     </row>
     <row r="44" spans="1:12" ht="30" thickBot="1">
       <c r="A44" s="4" t="s">
-        <v>707</v>
+        <v>807</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -4431,7 +4731,7 @@
     </row>
     <row r="45" spans="1:12" ht="30" thickBot="1">
       <c r="A45" s="4" t="s">
-        <v>708</v>
+        <v>808</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -4469,7 +4769,7 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" thickBot="1">
       <c r="A46" s="7" t="s">
-        <v>709</v>
+        <v>809</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -4507,7 +4807,7 @@
     </row>
     <row r="47" spans="1:12" ht="30" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>710</v>
+        <v>810</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -4545,7 +4845,7 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>711</v>
+        <v>811</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -4583,7 +4883,7 @@
     </row>
     <row r="49" spans="1:12" ht="30" thickBot="1">
       <c r="A49" s="7" t="s">
-        <v>712</v>
+        <v>812</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -4621,7 +4921,7 @@
     </row>
     <row r="50" spans="1:12" ht="30" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>713</v>
+        <v>813</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -4659,7 +4959,7 @@
     </row>
     <row r="51" spans="1:12" ht="30" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>714</v>
+        <v>814</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>

</xml_diff>